<commit_message>
Generated new groups file
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>nameAm~]N 8</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name^/$Qp </t>
-  </si>
-  <si>
-    <t>named}]Exza</t>
-  </si>
-  <si>
-    <t>name.</t>
+    <t>name"</t>
+  </si>
+  <si>
+    <t>nameD1vNOe[4@</t>
+  </si>
+  <si>
+    <t>name3Yr 6</t>
+  </si>
+  <si>
+    <t>namexu</t>
+  </si>
+  <si>
+    <t>namePD&gt; {x</t>
   </si>
 </sst>
 </file>

</xml_diff>